<commit_message>
Before sorting the map by sales
</commit_message>
<xml_diff>
--- a/Font Colors.xlsx
+++ b/Font Colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\go\src\listings_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958BA17A-9620-4CC3-BEB9-37CCA5E369F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB9D0B9-27A8-47C4-9D3B-DC74A52F097A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="3396" windowWidth="10656" windowHeight="8940" activeTab="1" xr2:uid="{4E89A022-6C1F-4EFD-B1A7-B6F2A51EC930}"/>
+    <workbookView xWindow="5448" yWindow="2496" windowWidth="10620" windowHeight="8928" activeTab="1" xr2:uid="{4E89A022-6C1F-4EFD-B1A7-B6F2A51EC930}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1982,7 +1982,7 @@
   <dimension ref="A2:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2090,14 +2090,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F763E75-5278-4782-B11E-E54DE28E2F8A}">
   <dimension ref="A1:BN694"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Changed mongostruct and other things
</commit_message>
<xml_diff>
--- a/Font Colors.xlsx
+++ b/Font Colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\go\src\listings_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB9D0B9-27A8-47C4-9D3B-DC74A52F097A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD490549-17A8-444B-90C6-009795227CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5448" yWindow="2496" windowWidth="10620" windowHeight="8928" activeTab="1" xr2:uid="{4E89A022-6C1F-4EFD-B1A7-B6F2A51EC930}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4E89A022-6C1F-4EFD-B1A7-B6F2A51EC930}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1971,7 +1971,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2090,8 +2090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F763E75-5278-4782-B11E-E54DE28E2F8A}">
   <dimension ref="A1:BN694"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>